<commit_message>
Ajout Adatateur usb aux commandes
</commit_message>
<xml_diff>
--- a/GestionDeProjet/Commandes.xlsx
+++ b/GestionDeProjet/Commandes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\s-cahors\Elsys\STAGES\22-9999-STAGE-ROBOT_AUTONOME_HOLONOME_V3\Robot_Surveillance_V3\GestionDeProjet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C95E6A9-C017-4593-B163-B91C1981F5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBCB9D3-A313-4395-A191-156AFCE14B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Farnell</t>
   </si>
@@ -97,6 +97,21 @@
   <si>
     <t>https://fr.farnell.com/en-FR/yageo/aes-acc-u96-jtag/pod-usb-jtag-uart/dp/2915522</t>
   </si>
+  <si>
+    <t>Creality 3D Printer Filament PLA 1.75mm 1KG Bobine,Matériaux d'impression 3D en filament- Noir</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/Creality-3D-Filament-1-75mm-imprimante/dp/B07HNWFQPN/ref=sr_1_5?__mk_fr_FR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;dchild=1&amp;keywords=filament%2Bpla%2B1.75%2Bcreality&amp;qid=1622454352&amp;sr=8-5&amp;th=1</t>
+  </si>
+  <si>
+    <t>JSAUX Câble Micro USB [1M+2M/Lot de 2]</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/JSAUX-Durable-t%C3%A9l%C3%A9phones-intelligents-Plus-Rouge/dp/B07V6CNQYC/ref=sr_1_11?__mk_fr_FR=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;keywords=cable%2Busb%2B2.0&amp;qid=1648643794&amp;s=computers&amp;sr=1-11&amp;th=1</t>
+  </si>
 </sst>
 </file>
 
@@ -107,7 +122,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-1]"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +155,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -292,7 +313,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -384,6 +405,24 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -668,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H985"/>
+  <dimension ref="A1:H988"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +759,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>18</v>
       </c>
@@ -745,7 +784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>19</v>
       </c>
@@ -778,8 +817,8 @@
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
     </row>
-    <row r="6" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -803,7 +842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -827,59 +866,85 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="8" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="35">
+        <v>23.59</v>
+      </c>
+      <c r="E9" s="36">
+        <v>1</v>
+      </c>
+      <c r="F9" s="37"/>
+      <c r="G9" s="22">
+        <f>D9*E9</f>
+        <v>23.59</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="33"/>
+      <c r="C10" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="35">
+        <v>9.99</v>
+      </c>
+      <c r="E10" s="36">
+        <v>2</v>
+      </c>
+      <c r="F10" s="37"/>
+      <c r="G10" s="22">
+        <f>D10*E10</f>
+        <v>19.98</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="9">
-        <f>SUM(G2:G7)</f>
-        <v>459.09000000000003</v>
+      <c r="G11" s="9">
+        <f>SUM(G2:G10)</f>
+        <v>502.66</v>
       </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
@@ -2842,34 +2907,34 @@
       <c r="H208" s="10"/>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A209" s="1"/>
-      <c r="B209" s="1"/>
-      <c r="C209" s="1"/>
-      <c r="D209" s="12"/>
-      <c r="E209" s="1"/>
-      <c r="F209" s="1"/>
-      <c r="G209" s="1"/>
-      <c r="H209" s="1"/>
+      <c r="A209" s="10"/>
+      <c r="B209" s="10"/>
+      <c r="C209" s="10"/>
+      <c r="D209" s="11"/>
+      <c r="E209" s="10"/>
+      <c r="F209" s="10"/>
+      <c r="G209" s="10"/>
+      <c r="H209" s="10"/>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A210" s="1"/>
-      <c r="B210" s="1"/>
-      <c r="C210" s="1"/>
-      <c r="D210" s="12"/>
-      <c r="E210" s="1"/>
-      <c r="F210" s="1"/>
-      <c r="G210" s="1"/>
-      <c r="H210" s="1"/>
+      <c r="A210" s="10"/>
+      <c r="B210" s="10"/>
+      <c r="C210" s="10"/>
+      <c r="D210" s="11"/>
+      <c r="E210" s="10"/>
+      <c r="F210" s="10"/>
+      <c r="G210" s="10"/>
+      <c r="H210" s="10"/>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A211" s="1"/>
-      <c r="B211" s="1"/>
-      <c r="C211" s="1"/>
-      <c r="D211" s="12"/>
-      <c r="E211" s="1"/>
-      <c r="F211" s="1"/>
-      <c r="G211" s="1"/>
-      <c r="H211" s="1"/>
+      <c r="A211" s="10"/>
+      <c r="B211" s="10"/>
+      <c r="C211" s="10"/>
+      <c r="D211" s="11"/>
+      <c r="E211" s="10"/>
+      <c r="F211" s="10"/>
+      <c r="G211" s="10"/>
+      <c r="H211" s="10"/>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
@@ -2962,13 +3027,34 @@
       <c r="H220" s="1"/>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A221" s="1"/>
+      <c r="B221" s="1"/>
+      <c r="C221" s="1"/>
       <c r="D221" s="12"/>
+      <c r="E221" s="1"/>
+      <c r="F221" s="1"/>
+      <c r="G221" s="1"/>
+      <c r="H221" s="1"/>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A222" s="1"/>
+      <c r="B222" s="1"/>
+      <c r="C222" s="1"/>
       <c r="D222" s="12"/>
+      <c r="E222" s="1"/>
+      <c r="F222" s="1"/>
+      <c r="G222" s="1"/>
+      <c r="H222" s="1"/>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A223" s="1"/>
+      <c r="B223" s="1"/>
+      <c r="C223" s="1"/>
       <c r="D223" s="12"/>
+      <c r="E223" s="1"/>
+      <c r="F223" s="1"/>
+      <c r="G223" s="1"/>
+      <c r="H223" s="1"/>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D224" s="12"/>
@@ -5255,6 +5341,15 @@
     </row>
     <row r="985" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D985" s="12"/>
+    </row>
+    <row r="986" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D986" s="12"/>
+    </row>
+    <row r="987" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D987" s="12"/>
+    </row>
+    <row r="988" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D988" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5262,7 +5357,10 @@
     <hyperlink ref="H3" r:id="rId2" xr:uid="{5E38454D-7637-4F23-AD81-C1DD33FB0D7C}"/>
     <hyperlink ref="H7" r:id="rId3" xr:uid="{9C1D1F7E-6881-4784-819F-F23EDB031D75}"/>
     <hyperlink ref="H4" r:id="rId4" xr:uid="{5754A4E9-BB56-4817-8667-AC8880DCFD0E}"/>
+    <hyperlink ref="H9" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="H10" r:id="rId6" xr:uid="{0ACCDFAE-1306-48A6-B87C-0B44E48C3401}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>